<commit_message>
removed mixed from aws
</commit_message>
<xml_diff>
--- a/comment_Analysis/anylizedchart.xlsx
+++ b/comment_Analysis/anylizedchart.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\issuecomments_analysis\comment_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloehebert/Documents/csc400/issuecomments_analysis/comment_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96085AB4-051B-4273-B445-D3EE8A95AD85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="15" windowWidth="26025" windowHeight="17610" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="1420" windowWidth="25600" windowHeight="15540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Watson" sheetId="1" r:id="rId1"/>
@@ -19,11 +18,11 @@
     <sheet name="Microsoft" sheetId="4" r:id="rId4"/>
     <sheet name="Google15" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
   <si>
     <t>Positive</t>
   </si>
@@ -65,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve"> mismatch: 2776</t>
-  </si>
-  <si>
-    <t>Mixed</t>
   </si>
   <si>
     <t>Mismatches</t>
@@ -139,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,7 +663,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42" xr:uid="{52DB03E6-9F42-43C3-B1EE-445D4608E39C}"/>
+    <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -688,7 +684,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -825,7 +821,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -852,12 +848,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1856</c:v>
+                  <c:v>1856.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3195-4A7A-99CD-9AF64395D74E}"/>
             </c:ext>
@@ -925,7 +921,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -952,12 +948,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2072</c:v>
+                  <c:v>2072.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3195-4A7A-99CD-9AF64395D74E}"/>
             </c:ext>
@@ -1025,7 +1021,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1052,12 +1048,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1603</c:v>
+                  <c:v>1603.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3195-4A7A-99CD-9AF64395D74E}"/>
             </c:ext>
@@ -1073,11 +1069,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1091706112"/>
-        <c:axId val="1090986112"/>
+        <c:axId val="-2084329376"/>
+        <c:axId val="-2084326048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1091706112"/>
+        <c:axId val="-2084329376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1090986112"/>
+        <c:crossAx val="-2084326048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1128,7 +1124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1090986112"/>
+        <c:axId val="-2084326048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1091706112"/>
+        <c:crossAx val="-2084329376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1224,14 +1220,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1267,7 +1263,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1311,6 +1307,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1347,10 +1344,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.0555555555555555E-2"/>
-          <c:y val="0.17374999999999999"/>
-          <c:w val="0.93888888888888888"/>
-          <c:h val="0.71818642461358995"/>
+          <c:x val="0.0305555555555556"/>
+          <c:y val="0.17375"/>
+          <c:w val="0.938888888888889"/>
+          <c:h val="0.71818642461359"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1383,7 +1380,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-C729-4E18-9EC0-21CB66FA7AB3}"/>
               </c:ext>
@@ -1404,7 +1401,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-C729-4E18-9EC0-21CB66FA7AB3}"/>
               </c:ext>
@@ -1445,8 +1442,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1488,18 +1486,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1313</c:v>
+                  <c:v>1313.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3267</c:v>
+                  <c:v>3267.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1289</c:v>
+                  <c:v>1289.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-C729-4E18-9EC0-21CB66FA7AB3}"/>
             </c:ext>
@@ -1516,11 +1514,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="1495297152"/>
-        <c:axId val="1509232576"/>
+        <c:axId val="-2069142000"/>
+        <c:axId val="-2069138528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1495297152"/>
+        <c:axId val="-2069142000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1509232576"/>
+        <c:crossAx val="-2069138528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1509232576"/>
+        <c:axId val="-2069138528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,7 +1593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1495297152"/>
+        <c:crossAx val="-2069142000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1609,14 +1607,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1652,7 +1650,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1695,8 +1693,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17098361272176221"/>
-          <c:y val="2.8950542822677925E-2"/>
+          <c:x val="0.170983612721762"/>
+          <c:y val="0.0289505428226779"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1735,10 +1733,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.2581741235833899E-2"/>
-          <c:y val="0.13885947046843178"/>
-          <c:w val="0.88607458951352014"/>
-          <c:h val="0.75442660807928541"/>
+          <c:x val="0.0725817412358339"/>
+          <c:y val="0.138859470468432"/>
+          <c:w val="0.88607458951352"/>
+          <c:h val="0.754426608079285"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1771,7 +1769,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-B9E2-47FA-8E8A-0AAD09445EB8}"/>
               </c:ext>
@@ -1790,7 +1788,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-B9E2-47FA-8E8A-0AAD09445EB8}"/>
               </c:ext>
@@ -1809,7 +1807,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-B9E2-47FA-8E8A-0AAD09445EB8}"/>
               </c:ext>
@@ -1853,8 +1851,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1877,7 +1876,7 @@
             <c:strRef>
               <c:f>AWS!$A$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Positive</c:v>
                 </c:pt>
@@ -1886,9 +1885,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Neutral</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mixed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1900,21 +1896,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1648</c:v>
+                  <c:v>1648.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1552</c:v>
+                  <c:v>1552.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2583</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>86</c:v>
+                  <c:v>2583.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-B9E2-47FA-8E8A-0AAD09445EB8}"/>
             </c:ext>
@@ -1931,11 +1924,11 @@
         </c:dLbls>
         <c:gapWidth val="85"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2078799072"/>
-        <c:axId val="-2078795984"/>
+        <c:axId val="-2069076128"/>
+        <c:axId val="-2069072928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2078799072"/>
+        <c:axId val="-2069076128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,7 +1971,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078795984"/>
+        <c:crossAx val="-2069072928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1986,7 +1979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2078795984"/>
+        <c:axId val="-2069072928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,7 +2030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078799072"/>
+        <c:crossAx val="-2069076128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2087,7 +2080,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2126,6 +2119,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2188,7 +2182,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-B381-41D5-B5AC-A7D1F91F675B}"/>
               </c:ext>
@@ -2209,7 +2203,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-B381-41D5-B5AC-A7D1F91F675B}"/>
               </c:ext>
@@ -2250,8 +2244,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2293,18 +2288,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1895</c:v>
+                  <c:v>1895.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2438</c:v>
+                  <c:v>2438.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1535</c:v>
+                  <c:v>1535.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B381-41D5-B5AC-A7D1F91F675B}"/>
             </c:ext>
@@ -2321,11 +2316,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="28302943"/>
-        <c:axId val="671599055"/>
+        <c:axId val="-2074950064"/>
+        <c:axId val="-2074946592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="28302943"/>
+        <c:axId val="-2074950064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2382,7 +2377,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="671599055"/>
+        <c:crossAx val="-2074946592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2390,7 +2385,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="671599055"/>
+        <c:axId val="-2074946592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2395,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="28302943"/>
+        <c:crossAx val="-2074950064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2414,14 +2409,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2457,7 +2452,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2496,6 +2491,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2532,10 +2528,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.0555555555555555E-2"/>
-          <c:y val="0.19226851851851851"/>
-          <c:w val="0.93888888888888888"/>
-          <c:h val="0.71818642461358995"/>
+          <c:x val="0.0305555555555556"/>
+          <c:y val="0.192268518518518"/>
+          <c:w val="0.938888888888889"/>
+          <c:h val="0.71818642461359"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2568,7 +2564,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-E2D8-444E-88A4-6672B2AD9A17}"/>
               </c:ext>
@@ -2587,7 +2583,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-E2D8-444E-88A4-6672B2AD9A17}"/>
               </c:ext>
@@ -2606,7 +2602,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-E2D8-444E-88A4-6672B2AD9A17}"/>
               </c:ext>
@@ -2647,8 +2643,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2690,18 +2687,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1450</c:v>
+                  <c:v>1450.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3049</c:v>
+                  <c:v>3049.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1370</c:v>
+                  <c:v>1370.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E2D8-444E-88A4-6672B2AD9A17}"/>
             </c:ext>
@@ -2718,11 +2715,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="718252847"/>
-        <c:axId val="551360767"/>
+        <c:axId val="-2085119968"/>
+        <c:axId val="-2071342320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="718252847"/>
+        <c:axId val="-2085119968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551360767"/>
+        <c:crossAx val="-2071342320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2787,7 +2784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551360767"/>
+        <c:axId val="-2071342320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2797,7 +2794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="718252847"/>
+        <c:crossAx val="-2085119968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2811,14 +2808,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5635,7 +5632,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283FFE59-93A5-4CD7-BC36-CCF5CF6DB08A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{283FFE59-93A5-4CD7-BC36-CCF5CF6DB08A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5676,7 +5673,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0B8BB7D-A3BA-457B-AD52-E6B0E889C162}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B0B8BB7D-A3BA-457B-AD52-E6B0E889C162}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5719,7 +5716,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45126E63-A84A-4D74-B299-0C7914E4D3A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45126E63-A84A-4D74-B299-0C7914E4D3A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5762,7 +5759,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E963CB41-3E83-42F3-B3BF-CC64C5FF4D31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E963CB41-3E83-42F3-B3BF-CC64C5FF4D31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5803,7 +5800,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A346DC-A0A3-4D19-A16E-62A978508B33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55A346DC-A0A3-4D19-A16E-62A978508B33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5822,19 +5819,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6133,46 +6117,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1856</v>
       </c>
@@ -6198,7 +6182,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6209,7 +6193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1128</v>
       </c>
@@ -6220,27 +6204,27 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -6264,7 +6248,7 @@
         <v>0.66756032171581769</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -6288,7 +6272,7 @@
         <v>0.47969861866889918</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -6319,21 +6303,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0539D62-1123-44DB-B31E-94BB09F0BDF8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6347,22 +6331,22 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1313</v>
       </c>
@@ -6392,7 +6376,7 @@
         <v>0.56549139839890994</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -6400,7 +6384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -6411,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1128</v>
       </c>
@@ -6422,27 +6406,27 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -6466,7 +6450,7 @@
         <v>0.43916427693568216</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -6490,7 +6474,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -6521,16 +6505,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CDE4AF-1830-4253-8F52-C0AE11C10105}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6540,22 +6524,20 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1648</v>
       </c>
@@ -6565,22 +6547,18 @@
       <c r="C2" s="1">
         <v>2583</v>
       </c>
-      <c r="D2" s="1">
-        <v>86</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1">
         <v>5869</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
-        <v>1961</v>
+        <v>1906</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1">
-        <v>0.66587152836939856</v>
-      </c>
+      <c r="I2" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -6597,7 +6575,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1128</v>
       </c>
@@ -6616,30 +6594,30 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -6649,20 +6627,23 @@
       <c r="C13" s="1">
         <v>665</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
+        <f>B13/(B13+C13)</f>
         <v>0.59599027946537064</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
+        <f>B13/A6</f>
         <v>0.86968085106382975</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <f>2*D13*E13/(D13+E13)</f>
         <v>0.70728190338860852</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -6672,37 +6653,43 @@
       <c r="C14" s="1">
         <v>967</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
+        <f t="shared" ref="D14:D15" si="0">B14/(B14+C14)</f>
         <v>0.35960264900662253</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
+        <f>B14/B6</f>
         <v>0.69083969465648853</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
+        <f t="shared" ref="F14:F15" si="1">2*D14*E14/(D14+E14)</f>
         <v>0.47299651567944245</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>2341</v>
+        <v>2396</v>
       </c>
       <c r="C15" s="1">
-        <v>240</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.90701278574196043</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.59190897597977243</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.71634026927784566</v>
+        <v>271</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.89838770153730785</v>
+      </c>
+      <c r="E15">
+        <f>B15/C6</f>
+        <v>0.60581542351453854</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.72364844457867705</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -6715,18 +6702,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25D5216-405E-42BE-ADC7-CFD6DCA22D6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6735,22 +6722,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1895</v>
       </c>
@@ -6776,7 +6763,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -6787,7 +6774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1128</v>
       </c>
@@ -6798,27 +6785,27 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -6842,7 +6829,7 @@
         <v>0.6166060205094277</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -6862,11 +6849,11 @@
         <v>0.80788804071246823</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F17" si="1">2*D16*E16/(D16+E16)</f>
+        <f t="shared" ref="F16" si="1">2*D16*E16/(D16+E16)</f>
         <v>0.5471779405428695</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -6897,48 +6884,48 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929479FC-4410-4CAB-9BF6-B17C5E2D714E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1450</v>
       </c>
@@ -6964,7 +6951,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -6975,7 +6962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1128</v>
       </c>
@@ -6986,27 +6973,27 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -7030,7 +7017,7 @@
         <v>0.49495733126454616</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -7042,7 +7029,7 @@
         <v>937</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D16" si="0">B15/(C15+B15)</f>
+        <f t="shared" ref="D15" si="0">B15/(C15+B15)</f>
         <v>0.31605839416058396</v>
       </c>
       <c r="E15">
@@ -7054,7 +7041,7 @@
         <v>0.40166975881261602</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
micro and macro avg
</commit_message>
<xml_diff>
--- a/comment_Analysis/anylizedchart.xlsx
+++ b/comment_Analysis/anylizedchart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="1420" windowWidth="25600" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="10360" yWindow="460" windowWidth="23160" windowHeight="14100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Watson" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="37">
   <si>
     <t>Positive</t>
   </si>
@@ -131,14 +131,36 @@
   <si>
     <t xml:space="preserve"> Google15Mismatch</t>
   </si>
+  <si>
+    <t>Micro avg</t>
+  </si>
+  <si>
+    <t>Macro avg</t>
+  </si>
+  <si>
+    <t>False Negatives</t>
+  </si>
+  <si>
+    <t>Micro Avg</t>
+  </si>
+  <si>
+    <t>Macro Avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -578,52 +600,54 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -723,6 +747,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -823,6 +848,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -923,6 +949,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1023,6 +1050,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1069,11 +1097,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2084329376"/>
-        <c:axId val="-2084326048"/>
+        <c:axId val="-2143848288"/>
+        <c:axId val="-2098518288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2084329376"/>
+        <c:axId val="-2143848288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084326048"/>
+        <c:crossAx val="-2098518288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084326048"/>
+        <c:axId val="-2098518288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084329376"/>
+        <c:crossAx val="-2143848288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,6 +1217,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1514,11 +1543,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="-2069142000"/>
-        <c:axId val="-2069138528"/>
+        <c:axId val="-2097633808"/>
+        <c:axId val="-2101124400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069142000"/>
+        <c:axId val="-2097633808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069138528"/>
+        <c:crossAx val="-2101124400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +1612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069138528"/>
+        <c:axId val="-2101124400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,7 +1622,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069142000"/>
+        <c:crossAx val="-2097633808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,7 +1931,7 @@
                   <c:v>1552.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2583.0</c:v>
+                  <c:v>2669.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1924,11 +1953,11 @@
         </c:dLbls>
         <c:gapWidth val="85"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2069076128"/>
-        <c:axId val="-2069072928"/>
+        <c:axId val="-2097559920"/>
+        <c:axId val="-2097556528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069076128"/>
+        <c:axId val="-2097559920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,7 +2000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069072928"/>
+        <c:crossAx val="-2097556528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1979,7 +2008,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069072928"/>
+        <c:axId val="-2097556528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069076128"/>
+        <c:crossAx val="-2097559920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2316,11 +2345,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="-2074950064"/>
-        <c:axId val="-2074946592"/>
+        <c:axId val="-2097490592"/>
+        <c:axId val="-2097487104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074950064"/>
+        <c:axId val="-2097490592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,7 +2406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074946592"/>
+        <c:crossAx val="-2097487104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2385,7 +2414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074946592"/>
+        <c:axId val="-2097487104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2395,7 +2424,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074950064"/>
+        <c:crossAx val="-2097490592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2715,11 +2744,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="-2085119968"/>
-        <c:axId val="-2071342320"/>
+        <c:axId val="-2097445216"/>
+        <c:axId val="-2097441728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2085119968"/>
+        <c:axId val="-2097445216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2776,7 +2805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071342320"/>
+        <c:crossAx val="-2097441728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2784,7 +2813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071342320"/>
+        <c:axId val="-2097441728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2794,7 +2823,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085119968"/>
+        <c:crossAx val="-2097445216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5632,7 +5661,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{283FFE59-93A5-4CD7-BC36-CCF5CF6DB08A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{283FFE59-93A5-4CD7-BC36-CCF5CF6DB08A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5673,7 +5702,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B0B8BB7D-A3BA-457B-AD52-E6B0E889C162}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0B8BB7D-A3BA-457B-AD52-E6B0E889C162}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5716,7 +5745,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45126E63-A84A-4D74-B299-0C7914E4D3A6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45126E63-A84A-4D74-B299-0C7914E4D3A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5759,7 +5788,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E963CB41-3E83-42F3-B3BF-CC64C5FF4D31}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E963CB41-3E83-42F3-B3BF-CC64C5FF4D31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5800,7 +5829,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55A346DC-A0A3-4D19-A16E-62A978508B33}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A346DC-A0A3-4D19-A16E-62A978508B33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6118,10 +6147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6296,6 +6325,38 @@
         <v>0.65107018417122953</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <f>(B8+B9+B10)/(C8+C9+C10+B8+B9+B10)</f>
+        <v>0.6384017356716688</v>
+      </c>
+      <c r="E11">
+        <v>0.6384017356716688</v>
+      </c>
+      <c r="F11">
+        <v>0.6384017356716688</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:E12" si="2">(D8+D9+D10)/3</f>
+        <v>0.61366796674920454</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0.70268908907741467</v>
+      </c>
+      <c r="F12">
+        <f>(F8+F9+F10)/3</f>
+        <v>0.5994430415186488</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6304,10 +6365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6498,6 +6559,38 @@
         <v>0.65549709221822205</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <f>(B13+B14+B15)/(C13+C14+C15+B13+B14+B15)</f>
+        <v>0.56534332935764187</v>
+      </c>
+      <c r="E16">
+        <v>0.56534332935764187</v>
+      </c>
+      <c r="F16">
+        <v>0.56534332935764187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:E17" si="2">(D13+D14+D15)/3</f>
+        <v>0.48489944938115742</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0.53388335328123271</v>
+      </c>
+      <c r="F17">
+        <f>(F13+F14+F15)/3</f>
+        <v>0.49822045638463469</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6506,10 +6599,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6545,7 +6638,7 @@
         <v>1552</v>
       </c>
       <c r="C2" s="1">
-        <v>2583</v>
+        <v>2669</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1">
@@ -6613,8 +6706,10 @@
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -6694,6 +6789,38 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <f>(B13+B14+B15)/(B13+B14+B15+C13+C14+C15)</f>
+        <v>0.67319251245062683</v>
+      </c>
+      <c r="E16">
+        <v>0.67319251245062683</v>
+      </c>
+      <c r="F16">
+        <v>0.67319251245062683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <f>(D13+D14+D15)/3</f>
+        <v>0.61799354333643375</v>
+      </c>
+      <c r="E17">
+        <f>(E13+E14+E15)/3</f>
+        <v>0.72211198974495228</v>
+      </c>
+      <c r="F17">
+        <f>(F13+F14+F15)/3</f>
+        <v>0.63464228788224264</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6703,10 +6830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6875,6 +7002,38 @@
       <c r="F17">
         <f>2*D17*E17/(D17+E17)</f>
         <v>0.67042077272016265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <f>(B15+B16+B17)/(B15+B16+B17+C15+C16+C17)</f>
+        <v>0.63224267211997276</v>
+      </c>
+      <c r="E18">
+        <v>0.63224267211997276</v>
+      </c>
+      <c r="F18">
+        <v>0.63224267211997298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:E19" si="2">(D15+D16+D17)/3</f>
+        <v>0.59483351396311568</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.72532498010628521</v>
+      </c>
+      <c r="F19">
+        <f>(F15+F16+F17)/3</f>
+        <v>0.61140157792415328</v>
       </c>
     </row>
   </sheetData>
@@ -6885,10 +7044,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7065,6 +7224,38 @@
         <v>0.65276984580239861</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <f>(B14+B15+B16)/(B14+B15+B16+C14+C15+C16)</f>
+        <v>0.57198841369909692</v>
+      </c>
+      <c r="E17">
+        <v>0.57198841369909692</v>
+      </c>
+      <c r="F17">
+        <v>0.57198841369909692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:E18" si="2">(D14+D15+D16)/3</f>
+        <v>0.50193747062376959</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.56483198352205644</v>
+      </c>
+      <c r="F18">
+        <f>(F14+F15+F16)/3</f>
+        <v>0.51646564529318695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>